<commit_message>
conditional routing : employee / admin
</commit_message>
<xml_diff>
--- a/src/assets/template/template.xlsx
+++ b/src/assets/template/template.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivam.sharma01\Desktop\mixed folder\Project\FreshVisitor\src\assets\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>SNO</t>
   </si>
@@ -42,15 +38,70 @@
   </si>
   <si>
     <t>NAME</t>
+  </si>
+  <si>
+    <t>VISITOR_TYPE</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Interviewee</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>VIP</t>
+  </si>
+  <si>
+    <t>New Joinee</t>
+  </si>
+  <si>
+    <t>Conference Attendee</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>Visitor</t>
+  </si>
+  <si>
+    <t>Visitor Type</t>
+  </si>
+  <si>
+    <t>Unique Id Type</t>
+  </si>
+  <si>
+    <t>Supported Values</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -77,8 +128,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,7 +192,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -174,7 +227,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -351,21 +404,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
@@ -374,7 +427,7 @@
     <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -392,10 +445,93 @@
       </c>
       <c r="F1" t="s">
         <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="21">
+      <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
unique id type dropdown values
</commit_message>
<xml_diff>
--- a/src/assets/template/template.xlsx
+++ b/src/assets/template/template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>SNO</t>
   </si>
@@ -77,6 +77,15 @@
   </si>
   <si>
     <t>Supported Values</t>
+  </si>
+  <si>
+    <t>Adharcard</t>
+  </si>
+  <si>
+    <t>Pancard</t>
+  </si>
+  <si>
+    <t>Passport</t>
   </si>
 </sst>
 </file>
@@ -404,7 +413,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -458,76 +467,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="21">
+    <row r="1" spans="1:2" ht="21">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+    <row r="7" spans="1:2">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
+    <row r="8" spans="1:2">
+      <c r="B8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
+    <row r="9" spans="1:2">
+      <c r="B9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
+    <row r="11" spans="1:2">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="B20" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>